<commit_message>
ajout dto et debut profile
</commit_message>
<xml_diff>
--- a/ProjetFilRouge/JeuxDeDonnees.xlsx
+++ b/ProjetFilRouge/JeuxDeDonnees.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Afpa\Repo_CDA_Consil_Anthony\90 - Fil rouge\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Developpement_Web\CDAQuentin\90 - Fil Rouge\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B017BB94-5F80-4FA1-8609-35A12DFA1DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{3A0D7E22-9474-442D-B693-53EAC14EB9DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jeux de données" sheetId="1" r:id="rId1"/>
     <sheet name="Script Jeux de données" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -425,12 +424,6 @@
     <t>Script du jeux de données.</t>
   </si>
   <si>
-    <t>INSERT INTO `adresses` (`IdAdresse`, `emailAdresse`, `telMobile`, `telFixe`, `adresse`, `province`, `complementAdresse`, `IdVille`) VALUES (2, 'Martine.Poix@Afpa.fr', '06080502', '0328569565', '96 rue de l\'eglise ', 'Nord', '59380 socx', 1);</t>
-  </si>
-  <si>
-    <t>INSERT INTO `adresses` (`IdAdresse`, `emailAdresse`, `telMobile`, `telFixe`, `adresse`, `province`, `complementAdresse`, `IdVille`) VALUES (1, 'Maxance@Bootstrap.com', '0602030203', '0328569569', '58 rue de l\'afpa ', 'Nord', '59240 dunkerque', 1);</t>
-  </si>
-  <si>
     <t>INSERT INTO `approvisionnements` (`IdApprovisionnement`, `IdProduit`, `IdFournisseur`, `refFournisseur`) VALUES (1, 3, 2, '15252');</t>
   </si>
   <si>
@@ -542,12 +535,6 @@
     <t>INSERT INTO `rubriques` (`IdRubrique`, `libelleRubrique`, `IdRubriqueMere`) VALUES (1, 'Corde', NULL);</t>
   </si>
   <si>
-    <t>INSERT INTO `rubriques` (`IdRubrique`, `libelleRubrique`, `IdRubriqueMere`) VALUES (3, 'Percussion', NULL);</t>
-  </si>
-  <si>
-    <t>INSERT INTO `rubriques` (`IdRubrique`, `libelleRubrique`, `IdRubriqueMere`) VALUES (2, 'Vent ', NULL);</t>
-  </si>
-  <si>
     <t>INSERT INTO `tva` (`IdTVA`, `tauxTVA`) VALUES (1, 20);</t>
   </si>
   <si>
@@ -570,12 +557,24 @@
   </si>
   <si>
     <t>INSERT INTO `villes` (`IdVille`, `libelleVIlle`, `codePostal`, `IdPays`) VALUES (3, 'Mogadiscio', '6369', 4);</t>
+  </si>
+  <si>
+    <t>INSERT INTO `rubriques` (`IdRubrique`, `libelleRubrique`, `IdRubriqueMere`) VALUES (2, 'Vent ', 1);</t>
+  </si>
+  <si>
+    <t>INSERT INTO `rubriques` (`IdRubrique`, `libelleRubrique`, `IdRubriqueMere`) VALUES (3, 'Percussion', 2);</t>
+  </si>
+  <si>
+    <t>INSERT INTO `adresses` (`IdAdresse`, `emailAdresse`, `telMobile`, `telFixe`, `adressePostale`, `province`, `complementAdresse`, `IdVille`) VALUES (1, 'Maxance@Bootstrap.com', '0602030203', '0328569569', '58 rue de l\'afpa ', 'Nord', '59240 dunkerque', 1);</t>
+  </si>
+  <si>
+    <t>INSERT INTO `adresses` (`IdAdresse`, `emailAdresse`, `telMobile`, `telFixe`, `adressePostale`, `province`, `complementAdresse`, `IdVille`) VALUES (2, 'Martine.Poix@Afpa.fr', '06080502', '0328569565', '96 rue de l\'eglise ', 'Nord', '59380 socx', 1);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1227,150 +1226,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1386,6 +1241,150 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1715,14 +1714,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67BD8EF-727D-4FAD-959F-91C9F0BE888D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
@@ -1780,34 +1779,34 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="112" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="106"/>
+      <c r="C2" s="113"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="107" t="s">
+      <c r="E2" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="109"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="116"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="110" t="s">
+      <c r="K2" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="112"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="119"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="113" t="s">
+      <c r="Q2" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="114"/>
-      <c r="S2" s="114"/>
-      <c r="T2" s="114"/>
-      <c r="U2" s="115"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="122"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
@@ -2132,31 +2131,31 @@
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="84"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="91"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="116" t="s">
+      <c r="G11" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="117"/>
+      <c r="H11" s="124"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="73" t="s">
+      <c r="J11" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="75"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="82"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="118" t="s">
+      <c r="O11" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="P11" s="119"/>
-      <c r="Q11" s="119"/>
-      <c r="R11" s="120"/>
+      <c r="P11" s="126"/>
+      <c r="Q11" s="126"/>
+      <c r="R11" s="127"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
@@ -2462,28 +2461,28 @@
     </row>
     <row r="20" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="81"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="88"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="82" t="s">
+      <c r="K20" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-      <c r="N20" s="84"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="90"/>
+      <c r="N20" s="91"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="85" t="s">
+      <c r="P20" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="Q20" s="86"/>
+      <c r="Q20" s="93"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
@@ -2812,29 +2811,29 @@
     </row>
     <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="87" t="s">
+      <c r="B29" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="89"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="96"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="90" t="s">
+      <c r="G29" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="H29" s="91"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
-      <c r="K29" s="91"/>
-      <c r="L29" s="91"/>
-      <c r="M29" s="91"/>
-      <c r="N29" s="92"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="98"/>
+      <c r="K29" s="98"/>
+      <c r="L29" s="98"/>
+      <c r="M29" s="98"/>
+      <c r="N29" s="99"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="76" t="s">
+      <c r="P29" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="Q29" s="77"/>
-      <c r="R29" s="78"/>
+      <c r="Q29" s="84"/>
+      <c r="R29" s="85"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
@@ -3132,34 +3131,34 @@
     </row>
     <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="93" t="s">
+      <c r="B37" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="95"/>
+      <c r="C37" s="101"/>
+      <c r="D37" s="101"/>
+      <c r="E37" s="102"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="96" t="s">
+      <c r="G37" s="103" t="s">
         <v>64</v>
       </c>
-      <c r="H37" s="97"/>
+      <c r="H37" s="104"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="98" t="s">
+      <c r="J37" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="K37" s="99"/>
-      <c r="L37" s="99"/>
-      <c r="M37" s="100"/>
+      <c r="K37" s="106"/>
+      <c r="L37" s="106"/>
+      <c r="M37" s="107"/>
       <c r="N37" s="1"/>
-      <c r="O37" s="101" t="s">
+      <c r="O37" s="108" t="s">
         <v>70</v>
       </c>
-      <c r="P37" s="102"/>
+      <c r="P37" s="109"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="103" t="s">
+      <c r="R37" s="110" t="s">
         <v>72</v>
       </c>
-      <c r="S37" s="104"/>
+      <c r="S37" s="111"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
@@ -3408,14 +3407,14 @@
     </row>
     <row r="44" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="B44" s="73" t="s">
+      <c r="B44" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="75"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="81"/>
+      <c r="G44" s="82"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -3483,7 +3482,7 @@
       <c r="D46" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="E46" s="123" t="s">
+      <c r="E46" s="75" t="s">
         <v>80</v>
       </c>
       <c r="F46" s="60">
@@ -3517,13 +3516,13 @@
       <c r="C47" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="121" t="s">
+      <c r="D47" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="124" t="s">
+      <c r="E47" s="76" t="s">
         <v>84</v>
       </c>
-      <c r="F47" s="122">
+      <c r="F47" s="74">
         <v>1212</v>
       </c>
       <c r="G47" s="59">
@@ -3961,267 +3960,267 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C5433C-E3DB-4F3F-B144-615AE1D80057}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="250.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="79" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="126" t="s">
-        <v>131</v>
+      <c r="B20" s="78" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="126" t="s">
-        <v>130</v>
+      <c r="B21" s="78" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="125" t="s">
-        <v>171</v>
+      <c r="B41" s="77" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="125" t="s">
-        <v>172</v>
+      <c r="B42" s="77" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>